<commit_message>
fertig bis auf die Bilder für das IPhone
</commit_message>
<xml_diff>
--- a/Zeit/Zeit-benötigt.xlsx
+++ b/Zeit/Zeit-benötigt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Website-files\Zeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8085EA6F-4EB7-4BC7-AE21-5D4AD074441F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4B47E3-858B-4FB7-B7AC-BFDF6F6A005D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +47,7 @@
     <t>Stunden</t>
   </si>
   <si>
-    <t>1*24</t>
+    <t>2*24</t>
   </si>
 </sst>
 </file>
@@ -101,13 +100,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A2:D31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A2:D32">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Von"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Bis"/>
@@ -502,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E33"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,72 +908,88 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>0</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="B28" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C28" s="3">
         <v>43992</v>
       </c>
       <c r="D28" s="2">
         <f>SUM(Tabelle1[[#This Row],[Bis]]-Tabelle1[[#This Row],[Von]])</f>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>0</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>0.59375</v>
       </c>
       <c r="C29" s="3">
         <v>43993</v>
       </c>
       <c r="D29" s="2">
         <f>SUM(Tabelle1[[#This Row],[Bis]]-Tabelle1[[#This Row],[Von]])</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>0</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C30" s="3">
         <v>43994</v>
       </c>
       <c r="D30" s="2">
         <f>SUM(Tabelle1[[#This Row],[Bis]]-Tabelle1[[#This Row],[Von]])</f>
-        <v>0</v>
+        <v>1.736111111111116E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>0</v>
+        <v>0.66319444444444442</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="C31" s="3">
         <v>43995</v>
       </c>
       <c r="D31" s="2">
         <f>SUM(Tabelle1[[#This Row],[Bis]]-Tabelle1[[#This Row],[Von]])</f>
-        <v>0</v>
+        <v>1.0416666666666741E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43997</v>
+      </c>
       <c r="D32" s="2">
+        <f>SUM(Tabelle1[[#This Row],[Bis]]-Tabelle1[[#This Row],[Von]])</f>
+        <v>2.7777777777777679E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="2">
         <f>SUM(Tabelle1[[#Data],[#Totals],[Stunden]])</f>
-        <v>1.9097222222222241</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+        <v>2.0034722222222241</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>